<commit_message>
Add of the data in excel
</commit_message>
<xml_diff>
--- a/ProgettoDB/tabelleDB.xlsx
+++ b/ProgettoDB/tabelleDB.xlsx
@@ -1,33 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="143" documentId="7_{238DD747-6DD4-C440-8725-0057AF580E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2969969-614D-AD49-9EC7-BA4F391B7CF3}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\campusfc.dir.unibo.it\share\UtentiIngISI\studenti\alesja.delja\Documents\Basi di dati\DBFair\ProgettoDB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78B0347-8E47-40E9-ACD0-C5F3C4178AA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Visitatori" sheetId="1" r:id="rId1"/>
+    <sheet name="Aziende" sheetId="2" r:id="rId2"/>
+    <sheet name="Padiglioni" sheetId="3" r:id="rId3"/>
+    <sheet name="Spazi" sheetId="4" r:id="rId4"/>
+    <sheet name="Prodotti" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="198">
   <si>
     <t>codice fiscale</t>
   </si>
@@ -228,12 +225,410 @@
   </si>
   <si>
     <t>TRCTMS19R11C155Z</t>
+  </si>
+  <si>
+    <t>codiceAzienda</t>
+  </si>
+  <si>
+    <t>Denominazione</t>
+  </si>
+  <si>
+    <t>Specializzazione</t>
+  </si>
+  <si>
+    <t>codicePadiglione</t>
+  </si>
+  <si>
+    <t>specializzazione Richiesta</t>
+  </si>
+  <si>
+    <t>orarioApertura</t>
+  </si>
+  <si>
+    <t>orarioChiusura</t>
+  </si>
+  <si>
+    <t>giornoAperturaAreaBambini</t>
+  </si>
+  <si>
+    <t>numSpaziEsposizione</t>
+  </si>
+  <si>
+    <t>numSpaziEsposizioneOccupati</t>
+  </si>
+  <si>
+    <t>Stampanti</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>Robot</t>
+  </si>
+  <si>
+    <t>Elettromestici</t>
+  </si>
+  <si>
+    <t>Audio e Video</t>
+  </si>
+  <si>
+    <t>Telefonia</t>
+  </si>
+  <si>
+    <t>CD-DVD</t>
+  </si>
+  <si>
+    <t>Videosorveglianza</t>
+  </si>
+  <si>
+    <t>Arduino</t>
+  </si>
+  <si>
+    <t>Modellismo</t>
+  </si>
+  <si>
+    <t>ABREX</t>
+  </si>
+  <si>
+    <t>2 Emme Foto</t>
+  </si>
+  <si>
+    <t>Milk Audio Store</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>3DiTALY</t>
+  </si>
+  <si>
+    <t>Candy</t>
+  </si>
+  <si>
+    <t>Ignis</t>
+  </si>
+  <si>
+    <t>OCEAN</t>
+  </si>
+  <si>
+    <t>Smeg</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>Oppo</t>
+  </si>
+  <si>
+    <t>Philips</t>
+  </si>
+  <si>
+    <t>SiComputer</t>
+  </si>
+  <si>
+    <t>Asus</t>
+  </si>
+  <si>
+    <t>Acer</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Lenovo</t>
+  </si>
+  <si>
+    <t>DSE</t>
+  </si>
+  <si>
+    <t>AMELI SRL</t>
+  </si>
+  <si>
+    <t>NSC ITALIA</t>
+  </si>
+  <si>
+    <t>Robotecnica Srl.</t>
+  </si>
+  <si>
+    <t>Tekna Automazioni Srl.</t>
+  </si>
+  <si>
+    <t>ABL Automazione S.p.A.</t>
+  </si>
+  <si>
+    <t>Lettera</t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>codiceProdotto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prezzo </t>
+  </si>
+  <si>
+    <t>descrizione</t>
+  </si>
+  <si>
+    <t>codice Azienda</t>
+  </si>
+  <si>
+    <t>Supporto Aerografi Magnetico</t>
+  </si>
+  <si>
+    <t>Kit pneumatico lavorazione lamierati</t>
+  </si>
+  <si>
+    <t>CD STAR</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>Stampa su cd serigrafica</t>
+  </si>
+  <si>
+    <t>DJI RONIN 4D 4-AXIS CINECAM 8K COMBO</t>
+  </si>
+  <si>
+    <t>drone</t>
+  </si>
+  <si>
+    <t>GOXTREME BARRACUDA WP</t>
+  </si>
+  <si>
+    <t>action cam</t>
+  </si>
+  <si>
+    <t>Buchla Easel Command</t>
+  </si>
+  <si>
+    <t>Stampante HP LaserJet M209dw</t>
+  </si>
+  <si>
+    <t>stampante laser</t>
+  </si>
+  <si>
+    <t>Scanner Enterprise HP ScanJet Flow N7000 snw1</t>
+  </si>
+  <si>
+    <t>scanner</t>
+  </si>
+  <si>
+    <t>Macchina da stampa a bobina HP PageWide T250 HD</t>
+  </si>
+  <si>
+    <t>macchina da stampa industriali</t>
+  </si>
+  <si>
+    <t>FORM 3BL BASIC PACKAGE WITH SERVICE</t>
+  </si>
+  <si>
+    <t>Laser cutter</t>
+  </si>
+  <si>
+    <t>macchine a taglio laser</t>
+  </si>
+  <si>
+    <t>Stampa 3D</t>
+  </si>
+  <si>
+    <t>stampa dei vostri modelli in tempo reale</t>
+  </si>
+  <si>
+    <t>Uno Rev 3 Arduino</t>
+  </si>
+  <si>
+    <t>Leonardo with headers Arduino</t>
+  </si>
+  <si>
+    <t>Lavatrice RCSS149HMC-S</t>
+  </si>
+  <si>
+    <t>lavatrice a carica frontale</t>
+  </si>
+  <si>
+    <t>CANDY CRE H10A2DE-S asciugatrice</t>
+  </si>
+  <si>
+    <t>asciugatrice</t>
+  </si>
+  <si>
+    <t>CANDY CSTG 28TE/1-11</t>
+  </si>
+  <si>
+    <t>lavatrice a carica dall'alto</t>
+  </si>
+  <si>
+    <t>NFW 830 H IX</t>
+  </si>
+  <si>
+    <t>forno</t>
+  </si>
+  <si>
+    <t>REFRIGERATOR PFRC 400 S A+ WFS .</t>
+  </si>
+  <si>
+    <t>frigorifero</t>
+  </si>
+  <si>
+    <t>NO FROST REFRIG. MDD 550 NF BG A+</t>
+  </si>
+  <si>
+    <t>frigorifero SMEG FAB28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frigorifero </t>
+  </si>
+  <si>
+    <t>Frigo Snoopy</t>
+  </si>
+  <si>
+    <t>Frigo Topolino</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A12 (128 GB) Black</t>
+  </si>
+  <si>
+    <t>smartphone</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A32 Black</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S22 5G Black 128 GB</t>
+  </si>
+  <si>
+    <t>Apple iPhone 13 Pro 128 GB Argento</t>
+  </si>
+  <si>
+    <t>Apple Watch Nike Series 7 GPS 41mm Alluminio</t>
+  </si>
+  <si>
+    <t>apple watch</t>
+  </si>
+  <si>
+    <t>Apple 10.2-inch iPad 2021 Wi-Fi 64GB - SILVER</t>
+  </si>
+  <si>
+    <t>tablet</t>
+  </si>
+  <si>
+    <t>OnePlus 10 Pro 5G</t>
+  </si>
+  <si>
+    <t>Monitor Led 49" Philips</t>
+  </si>
+  <si>
+    <t>monitor pc</t>
+  </si>
+  <si>
+    <t>SI COMPUTER ACTIVA PC USATO</t>
+  </si>
+  <si>
+    <t>computer case</t>
+  </si>
+  <si>
+    <t>Asus 14" Zenbook Duo UX482EGR</t>
+  </si>
+  <si>
+    <t>portatile</t>
+  </si>
+  <si>
+    <t>ACER - CONCEPTD 300 CT300</t>
+  </si>
+  <si>
+    <t>ThinkPad X1 Carbon Gen 9</t>
+  </si>
+  <si>
+    <t>MINI SPEED DOME POE</t>
+  </si>
+  <si>
+    <t>telecamera autotracking</t>
+  </si>
+  <si>
+    <t>Kit Videosorveglianza Ultra AHD 4 Telecamere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">telecamera </t>
+  </si>
+  <si>
+    <t>Comelit</t>
+  </si>
+  <si>
+    <t>Sistemi di irrigazione con pannelli fotovoltaici</t>
+  </si>
+  <si>
+    <t>Scheda tecnica Aerogeneratore 30kW</t>
+  </si>
+  <si>
+    <t>Impianto di Produzione Contatori Gas</t>
+  </si>
+  <si>
+    <t>VINILE 12 pollici</t>
+  </si>
+  <si>
+    <t>pezzi modello auto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kit </t>
+  </si>
+  <si>
+    <t>vinile</t>
+  </si>
+  <si>
+    <t>disco</t>
+  </si>
+  <si>
+    <t>servizio di stampa in tempo reale</t>
+  </si>
+  <si>
+    <t>audio</t>
+  </si>
+  <si>
+    <t>stampante 3D</t>
+  </si>
+  <si>
+    <t>arduino</t>
+  </si>
+  <si>
+    <t>estrazione acqua</t>
+  </si>
+  <si>
+    <t>uso turbine</t>
+  </si>
+  <si>
+    <t>montaggio contatori</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -263,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -271,6 +666,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -587,20 +987,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0808F2E3-AED5-CE4A-9ACC-8C0FA42CDB28}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.05859375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.3125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.890625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.66015625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.609375" style="1"/>
+    <col min="1" max="1" width="22" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,7 +1017,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -634,7 +1034,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -651,7 +1051,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -668,7 +1068,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -685,7 +1085,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -702,7 +1102,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -719,7 +1119,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -736,7 +1136,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -753,7 +1153,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -770,7 +1170,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -787,7 +1187,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -804,7 +1204,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -821,7 +1221,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
@@ -838,7 +1238,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
@@ -855,7 +1255,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
@@ -872,7 +1272,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -889,7 +1289,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>55</v>
       </c>
@@ -906,7 +1306,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -923,7 +1323,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>61</v>
       </c>
@@ -940,7 +1340,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>66</v>
       </c>
@@ -960,4 +1360,1694 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14BC05F4-4AAB-4C78-92F9-F5FA5141C6FF}">
+  <dimension ref="A1:E38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D26627CC-5AA0-45F4-80B0-E09FCCE61EA5}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2">
+        <v>60</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E3" s="5">
+        <v>44687</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E5" s="5">
+        <v>44690</v>
+      </c>
+      <c r="F5">
+        <v>200</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E7" s="5">
+        <v>44688</v>
+      </c>
+      <c r="F7">
+        <v>500</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8">
+        <v>250</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E9" s="5">
+        <v>44689</v>
+      </c>
+      <c r="F9">
+        <v>300</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E11" s="4">
+        <v>44691</v>
+      </c>
+      <c r="F11">
+        <v>80</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6362A034-533F-4DC4-BE4F-A1B6CA3BAC49}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD2AFD86-F7EB-48A4-B6DD-0FC41B4FF034}">
+  <dimension ref="A1:E46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="7">
+        <v>20</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="7">
+        <v>15</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="7">
+        <v>40</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="7">
+        <v>20</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="7">
+        <v>20</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="7">
+        <v>11000</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="7">
+        <v>92</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="7">
+        <v>3280</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="7">
+        <v>200</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="7">
+        <v>250</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="7">
+        <v>20000</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" s="7">
+        <v>13000</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="7">
+        <v>10000</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="7">
+        <v>500</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="7">
+        <v>25</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" s="7">
+        <v>20</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" s="7">
+        <v>394</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" s="7">
+        <v>500</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" s="7">
+        <v>420</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" s="7">
+        <v>400</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="7">
+        <v>350</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="7">
+        <v>450</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C24" s="7">
+        <v>600</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25" s="7">
+        <v>550</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C26" s="7">
+        <v>550</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27" s="7">
+        <v>200</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C28" s="7">
+        <v>280</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C29" s="7">
+        <v>725</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C30" s="7">
+        <v>970</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C31" s="7">
+        <v>440</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" s="7">
+        <v>415</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E32">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="7">
+        <v>419</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C34" s="7">
+        <v>1126.6400000000001</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E34">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C35" s="7">
+        <v>50</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C36" s="7">
+        <v>1285</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E36">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C37" s="7">
+        <v>2140</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E37">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C38" s="7">
+        <v>2799</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E38">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C39" s="7">
+        <v>500</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C40" s="7">
+        <v>640</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E40">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C41" s="7">
+        <v>40</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E41">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C42" s="7">
+        <v>1000</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E42">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C43" s="7">
+        <v>1000</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E43">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C44" s="7">
+        <v>2000</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E44">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="6"/>
+    </row>
+    <row r="46" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>